<commit_message>
Fix bug in interpolating widths.
</commit_message>
<xml_diff>
--- a/geometry.xlsx
+++ b/geometry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvemo\Documents\my_stuff\Publication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvemo\Documents\my_stuff\Publication\flood-wave-propagation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF2E724-7933-4B59-833D-5E6F95026D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2212A6-61BF-4329-9D87-E012BE2338DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{698A3176-6DCE-4A7A-AF8C-646E8BD6C9FD}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{698A3176-6DCE-4A7A-AF8C-646E8BD6C9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sections - Copy" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Chainage</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>m</t>
-  </si>
-  <si>
-    <t>GERD</t>
   </si>
 </sst>
 </file>
@@ -941,7 +938,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,314 +979,270 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
+      <c r="A3" s="8">
+        <v>54</v>
       </c>
       <c r="B3">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>893</v>
-      </c>
-      <c r="D3" s="6">
-        <v>470.54</v>
+        <v>250</v>
+      </c>
+      <c r="D3" s="5">
+        <v>495</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B4">
-        <v>119822</v>
+        <v>16130</v>
       </c>
       <c r="C4" s="2">
-        <v>1475</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>758</v>
+      </c>
+      <c r="D4" s="6">
+        <v>488.16899999999998</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B5">
-        <v>119584</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2465</v>
-      </c>
-      <c r="D5" s="6">
-        <v>470.93700000000001</v>
-      </c>
+        <v>18907</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B6">
-        <v>118867</v>
+        <v>21875</v>
       </c>
       <c r="C6" s="2">
-        <v>4630</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>586</v>
+      </c>
+      <c r="D6" s="6">
+        <v>479.35700000000003</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>117882</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6034</v>
-      </c>
-      <c r="D7" s="6">
-        <v>474.52100000000002</v>
-      </c>
+        <v>24768</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B8">
-        <v>117166</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7145</v>
-      </c>
-      <c r="D8" s="6">
-        <v>474.089</v>
-      </c>
+        <v>27681</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B9">
-        <v>116164</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8118</v>
-      </c>
-      <c r="D9" s="6">
-        <v>477.23</v>
-      </c>
+        <v>30944</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B10">
-        <v>114957</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7073</v>
-      </c>
-      <c r="D10" s="6">
-        <v>474.80700000000002</v>
-      </c>
+        <v>33683</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B11">
-        <v>113586</v>
+        <v>36490</v>
       </c>
       <c r="C11" s="2">
-        <v>9084</v>
+        <v>696</v>
       </c>
       <c r="D11" s="6">
-        <v>473.11700000000002</v>
+        <v>476.92399999999998</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B12">
-        <v>112586</v>
-      </c>
-      <c r="C12" s="2">
-        <v>9539</v>
-      </c>
+        <v>39426</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="7"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B13">
-        <v>110472</v>
-      </c>
-      <c r="C13" s="2">
-        <v>6325</v>
-      </c>
-      <c r="D13" s="6">
-        <v>473.14699999999999</v>
-      </c>
+        <v>42169</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <v>109459</v>
-      </c>
-      <c r="C14" s="2">
-        <v>6982</v>
-      </c>
+        <v>45156</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="7"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>108517</v>
+        <v>48133</v>
       </c>
       <c r="C15" s="2">
-        <v>6294</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>976</v>
+      </c>
+      <c r="D15" s="6">
+        <v>472.95499999999998</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B16">
-        <v>107585</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5876</v>
-      </c>
-      <c r="D16" s="6">
-        <v>476.39400000000001</v>
-      </c>
+        <v>50144</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B17">
-        <v>105653</v>
-      </c>
-      <c r="C17" s="2">
-        <v>6559</v>
-      </c>
-      <c r="D17" s="6">
-        <v>475.39800000000002</v>
-      </c>
+        <v>51678</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B18">
-        <v>104135</v>
-      </c>
-      <c r="C18" s="2">
-        <v>7035</v>
-      </c>
+        <v>53787</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="7"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B19">
-        <v>102391</v>
-      </c>
-      <c r="C19" s="2">
-        <v>7443</v>
-      </c>
+        <v>55853</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="7"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>99287</v>
-      </c>
-      <c r="C20" s="2">
-        <v>5360</v>
-      </c>
+        <v>57734</v>
+      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="7"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B21">
-        <v>96892</v>
+        <v>59763</v>
       </c>
       <c r="C21" s="2">
-        <v>8279</v>
+        <v>1750</v>
       </c>
       <c r="D21" s="6">
-        <v>474.04199999999997</v>
+        <v>478.21100000000001</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B22">
-        <v>94519</v>
-      </c>
-      <c r="C22" s="2">
-        <v>5240</v>
-      </c>
+        <v>61719</v>
+      </c>
+      <c r="C22" s="2"/>
       <c r="D22" s="7"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>92330</v>
-      </c>
-      <c r="C23" s="2">
-        <v>5819</v>
-      </c>
-      <c r="D23" s="6">
-        <v>474.61399999999998</v>
-      </c>
+        <v>63696</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B24">
-        <v>90224</v>
-      </c>
-      <c r="C24" s="2">
-        <v>4861</v>
-      </c>
+        <v>65819</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="7"/>
       <c r="E24" s="1"/>
       <c r="H24" s="1"/>
@@ -1297,14 +1250,12 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>88014</v>
-      </c>
-      <c r="C25" s="2">
-        <v>5252</v>
-      </c>
+        <v>67854</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="7"/>
       <c r="E25" s="1"/>
       <c r="H25" s="1"/>
@@ -1312,16 +1263,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>84759</v>
+        <v>69937</v>
       </c>
       <c r="C26" s="2">
-        <v>3105</v>
+        <v>2397</v>
       </c>
       <c r="D26" s="6">
-        <v>476.16800000000001</v>
+        <v>476.40499999999997</v>
       </c>
       <c r="E26" s="1"/>
       <c r="H26" s="1"/>
@@ -1329,14 +1280,12 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B27">
-        <v>83016</v>
-      </c>
-      <c r="C27" s="2">
-        <v>2660</v>
-      </c>
+        <v>71312</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="7"/>
       <c r="E27" s="1"/>
       <c r="H27" s="1"/>
@@ -1344,29 +1293,29 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>80523</v>
+        <v>73780</v>
       </c>
       <c r="C28" s="2">
-        <v>2209</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>2610</v>
+      </c>
+      <c r="D28" s="6">
+        <v>476.85899999999998</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>77878</v>
-      </c>
-      <c r="C29" s="2">
-        <v>2152</v>
-      </c>
+        <v>75350</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
       <c r="H29" s="1"/>
@@ -1374,14 +1323,12 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>75350</v>
-      </c>
-      <c r="C30" s="2">
-        <v>3492</v>
-      </c>
+        <v>77878</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="7"/>
       <c r="E30" s="1"/>
       <c r="H30" s="1"/>
@@ -1389,31 +1336,25 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>73780</v>
-      </c>
-      <c r="C31" s="2">
-        <v>2610</v>
-      </c>
-      <c r="D31" s="6">
-        <v>476.85899999999998</v>
-      </c>
+        <v>80523</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B32">
-        <v>71312</v>
-      </c>
-      <c r="C32" s="2">
-        <v>2949</v>
-      </c>
+        <v>83016</v>
+      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="7"/>
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
@@ -1421,16 +1362,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>69937</v>
+        <v>84759</v>
       </c>
       <c r="C33" s="2">
-        <v>2397</v>
+        <v>3105</v>
       </c>
       <c r="D33" s="6">
-        <v>476.40499999999997</v>
+        <v>476.16800000000001</v>
       </c>
       <c r="E33" s="1"/>
       <c r="H33" s="1"/>
@@ -1438,14 +1379,12 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B34">
-        <v>67854</v>
-      </c>
-      <c r="C34" s="2">
-        <v>2347</v>
-      </c>
+        <v>88014</v>
+      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="7"/>
       <c r="E34" s="1"/>
       <c r="H34" s="1"/>
@@ -1453,14 +1392,12 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B35">
-        <v>65819</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1852</v>
-      </c>
+        <v>90224</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="7"/>
       <c r="E35" s="1"/>
       <c r="H35" s="1"/>
@@ -1468,29 +1405,29 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B36">
-        <v>63696</v>
+        <v>92330</v>
       </c>
       <c r="C36" s="2">
-        <v>1700</v>
-      </c>
-      <c r="D36" s="7"/>
+        <v>5819</v>
+      </c>
+      <c r="D36" s="6">
+        <v>474.61399999999998</v>
+      </c>
       <c r="E36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>61719</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1540</v>
-      </c>
+        <v>94519</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="7"/>
       <c r="E37" s="1"/>
       <c r="H37" s="1"/>
@@ -1498,16 +1435,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B38">
-        <v>59763</v>
+        <v>96892</v>
       </c>
       <c r="C38" s="2">
-        <v>1750</v>
+        <v>8279</v>
       </c>
       <c r="D38" s="6">
-        <v>478.21100000000001</v>
+        <v>474.04199999999997</v>
       </c>
       <c r="E38" s="1"/>
       <c r="H38" s="1"/>
@@ -1515,14 +1452,12 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B39">
-        <v>57734</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1651</v>
-      </c>
+        <v>99287</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="7"/>
       <c r="E39" s="1"/>
       <c r="H39" s="1"/>
@@ -1530,14 +1465,12 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B40">
-        <v>55853</v>
-      </c>
-      <c r="C40" s="2">
-        <v>2246</v>
-      </c>
+        <v>102391</v>
+      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="7"/>
       <c r="E40" s="1"/>
       <c r="H40" s="1"/>
@@ -1545,14 +1478,12 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B41">
-        <v>53787</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2559</v>
-      </c>
+        <v>104135</v>
+      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="7"/>
       <c r="E41" s="1"/>
       <c r="H41" s="1"/>
@@ -1560,61 +1491,59 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B42">
-        <v>51678</v>
+        <v>105653</v>
       </c>
       <c r="C42" s="2">
-        <v>2102</v>
-      </c>
-      <c r="D42" s="7"/>
+        <v>6559</v>
+      </c>
+      <c r="D42" s="6">
+        <v>475.39800000000002</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B43">
-        <v>50144</v>
+        <v>107585</v>
       </c>
       <c r="C43" s="2">
-        <v>1477</v>
-      </c>
-      <c r="D43" s="7"/>
+        <v>5876</v>
+      </c>
+      <c r="D43" s="6">
+        <v>476.39400000000001</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B44">
-        <v>48133</v>
-      </c>
-      <c r="C44" s="2">
-        <v>976</v>
-      </c>
-      <c r="D44" s="6">
-        <v>472.95499999999998</v>
-      </c>
+        <v>108517</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="7"/>
       <c r="E44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B45">
-        <v>45156</v>
-      </c>
-      <c r="C45" s="2">
-        <v>635</v>
-      </c>
+        <v>109459</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="7"/>
       <c r="E45" s="1"/>
       <c r="H45" s="1"/>
@@ -1622,29 +1551,29 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B46">
-        <v>42169</v>
+        <v>110472</v>
       </c>
       <c r="C46" s="2">
-        <v>622</v>
-      </c>
-      <c r="D46" s="7"/>
+        <v>6325</v>
+      </c>
+      <c r="D46" s="6">
+        <v>473.14699999999999</v>
+      </c>
       <c r="E46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="B47">
-        <v>39426</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1076</v>
-      </c>
+        <v>112586</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="7"/>
       <c r="E47" s="1"/>
       <c r="H47" s="1"/>
@@ -1652,16 +1581,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B48">
-        <v>36490</v>
+        <v>113586</v>
       </c>
       <c r="C48" s="2">
-        <v>696</v>
+        <v>9084</v>
       </c>
       <c r="D48" s="6">
-        <v>476.92399999999998</v>
+        <v>473.11700000000002</v>
       </c>
       <c r="E48" s="1"/>
       <c r="H48" s="1"/>
@@ -1669,125 +1598,123 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B49">
-        <v>33683</v>
+        <v>114957</v>
       </c>
       <c r="C49" s="2">
-        <v>772</v>
-      </c>
-      <c r="D49" s="7"/>
+        <v>7073</v>
+      </c>
+      <c r="D49" s="6">
+        <v>474.80700000000002</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="B50">
-        <v>30944</v>
+        <v>116164</v>
       </c>
       <c r="C50" s="2">
-        <v>864</v>
-      </c>
-      <c r="D50" s="7"/>
+        <v>8118</v>
+      </c>
+      <c r="D50" s="6">
+        <v>477.23</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B51">
-        <v>27681</v>
+        <v>117166</v>
       </c>
       <c r="C51" s="2">
-        <v>894</v>
-      </c>
-      <c r="D51" s="7"/>
+        <v>7145</v>
+      </c>
+      <c r="D51" s="6">
+        <v>474.089</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B52">
-        <v>24768</v>
+        <v>117882</v>
       </c>
       <c r="C52" s="2">
-        <v>1092</v>
-      </c>
-      <c r="D52" s="7"/>
+        <v>6034</v>
+      </c>
+      <c r="D52" s="6">
+        <v>474.52100000000002</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B53">
-        <v>21875</v>
-      </c>
-      <c r="C53" s="2">
-        <v>586</v>
-      </c>
-      <c r="D53" s="6">
-        <v>479.35700000000003</v>
-      </c>
+        <v>118867</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="7"/>
       <c r="E53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>18907</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1005</v>
-      </c>
-      <c r="D54" s="6"/>
+        <v>119584</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="6">
+        <v>470.93700000000001</v>
+      </c>
       <c r="E54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="B55">
-        <v>16130</v>
-      </c>
-      <c r="C55" s="2">
-        <v>758</v>
-      </c>
-      <c r="D55" s="6">
-        <v>488.16899999999998</v>
-      </c>
+        <v>119822</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="7"/>
       <c r="E55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>5</v>
+      <c r="A56" s="4">
+        <v>1</v>
       </c>
       <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56" s="2">
-        <v>250</v>
-      </c>
-      <c r="D56" s="5">
-        <v>495</v>
+        <v>120000</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="6">
+        <v>470.54</v>
       </c>
       <c r="E56" s="1"/>
       <c r="H56" s="1"/>
@@ -1892,6 +1819,9 @@
       <c r="K72" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D56">
+    <sortCondition descending="1" ref="A56"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>